<commit_message>
Dodati su testovii za otvaranje svih stranica
</commit_message>
<xml_diff>
--- a/src/main/resources/Data.xlsx
+++ b/src/main/resources/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\IdeaProjects\QaProjekat\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C68C76D6-170F-4244-8007-4C86FE83B135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6340FED0-31CF-443C-ADF4-E75EFE170AFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{FC03CCA5-9AE7-4DEA-931D-0B6A67AD7227}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{FC03CCA5-9AE7-4DEA-931D-0B6A67AD7227}"/>
   </bookViews>
   <sheets>
     <sheet name="URL" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>URLs</t>
   </si>
@@ -70,6 +70,21 @@
   </si>
   <si>
     <t>https://demoqa.com/browser-windows</t>
+  </si>
+  <si>
+    <t>Terms</t>
+  </si>
+  <si>
+    <t>Git</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>JS</t>
+  </si>
+  <si>
+    <t>Web</t>
   </si>
 </sst>
 </file>
@@ -444,7 +459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8053081C-7EE5-4660-96E5-B99BA227D072}">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -522,12 +537,40 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AC9521B-DBE1-4660-AD82-CBBB9A849AB0}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>